<commit_message>
Improving error message for assertoins in Calculation Coordinator
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/Lookups.xlsx
+++ b/CalculationCoordinator/Lookups.xlsx
@@ -423,12 +423,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -439,43 +439,43 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" width="9.10" max="6"/>
-    <col min="7" width="9.10" max="7"/>
-    <col min="4" width="9.10" max="4"/>
-    <col min="5" width="9.10" max="5"/>
-    <col min="2" width="9.10" max="2"/>
-    <col min="3" width="9.10" max="3"/>
-    <col min="1" width="9.10" max="1"/>
-    <col min="14" width="9.10" max="14"/>
-    <col min="15" width="9.10" max="15"/>
-    <col min="12" width="9.10" max="12"/>
-    <col min="13" width="9.10" max="13"/>
-    <col min="10" width="9.10" max="10"/>
-    <col min="11" width="9.10" max="11"/>
-    <col min="8" width="9.10" max="8"/>
-    <col min="9" width="9.10" max="9"/>
-    <col min="22" width="9.10" max="22"/>
-    <col min="23" width="9.10" max="23"/>
-    <col min="20" width="9.10" max="20"/>
-    <col min="21" width="9.10" max="21"/>
-    <col min="18" width="9.10" max="18"/>
-    <col min="19" width="9.10" max="19"/>
-    <col min="16" width="9.10" max="16"/>
-    <col min="17" width="9.10" max="17"/>
-    <col min="24" width="9.10" max="24"/>
+    <col max="23" min="23" width="9.10"/>
+    <col max="22" min="22" width="9.10"/>
+    <col max="21" min="21" width="9.10"/>
+    <col max="20" min="20" width="9.10"/>
+    <col max="19" min="19" width="9.10"/>
+    <col max="18" min="18" width="9.10"/>
+    <col max="17" min="17" width="9.10"/>
+    <col max="16" min="16" width="9.10"/>
+    <col max="24" min="24" width="9.10"/>
+    <col max="7" min="7" width="9.10"/>
+    <col max="6" min="6" width="9.10"/>
+    <col max="5" min="5" width="9.10"/>
+    <col max="4" min="4" width="9.10"/>
+    <col max="3" min="3" width="9.10"/>
+    <col max="2" min="2" width="9.10"/>
+    <col max="1" min="1" width="9.10"/>
+    <col max="15" min="15" width="9.10"/>
+    <col max="14" min="14" width="9.10"/>
+    <col max="13" min="13" width="9.10"/>
+    <col max="12" min="12" width="9.10"/>
+    <col max="11" min="11" width="9.10"/>
+    <col max="10" min="10" width="9.10"/>
+    <col max="9" min="9" width="9.10"/>
+    <col max="8" min="8" width="9.10"/>
   </cols>
   <sheetData>
-    <row spans="1:24" r="1">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -522,7 +522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row spans="1:24" r="2">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -593,7 +593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row spans="1:24" r="3">
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -664,7 +664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row spans="1:24" r="4">
+    <row r="4" spans="1:24">
       <c r="F4" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Fixed tests that utilize additional cut menus
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/Lookups.xlsx
+++ b/CalculationCoordinator/Lookups.xlsx
@@ -16,6 +16,8 @@
     <definedName name="cuts_historical">'Lookups'!$F$4:$F$4</definedName>
     <definedName name="cuts_2">'Lookups'!$F$5:$F$4</definedName>
     <definedName name="cuts_3">'Lookups'!$F$5:$F$4</definedName>
+    <definedName name="cuts_4">'Lookups'!$F$5:$F$4</definedName>
+    <definedName name="cuts_5">'Lookups'!$F$5:$F$4</definedName>
     <definedName name="default_menu">'Lookups'!$F$2:$F$1001</definedName>
     <definedName name="default_mapping">'Lookups'!$F$2:$G$1001</definedName>
     <definedName name="default_menu_start">'Lookups'!$F$2</definedName>
@@ -423,12 +425,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -439,40 +441,40 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="23" min="23" width="9.10"/>
-    <col max="22" min="22" width="9.10"/>
-    <col max="21" min="21" width="9.10"/>
-    <col max="20" min="20" width="9.10"/>
-    <col max="19" min="19" width="9.10"/>
-    <col max="18" min="18" width="9.10"/>
-    <col max="17" min="17" width="9.10"/>
-    <col max="16" min="16" width="9.10"/>
-    <col max="24" min="24" width="9.10"/>
-    <col max="7" min="7" width="9.10"/>
-    <col max="6" min="6" width="9.10"/>
-    <col max="5" min="5" width="9.10"/>
-    <col max="4" min="4" width="9.10"/>
-    <col max="3" min="3" width="9.10"/>
-    <col max="2" min="2" width="9.10"/>
-    <col max="1" min="1" width="9.10"/>
-    <col max="15" min="15" width="9.10"/>
-    <col max="14" min="14" width="9.10"/>
-    <col max="13" min="13" width="9.10"/>
-    <col max="12" min="12" width="9.10"/>
-    <col max="11" min="11" width="9.10"/>
-    <col max="10" min="10" width="9.10"/>
-    <col max="9" min="9" width="9.10"/>
-    <col max="8" min="8" width="9.10"/>
+    <col min="7" width="9.10" max="7"/>
+    <col min="6" width="9.10" max="6"/>
+    <col min="5" width="9.10" max="5"/>
+    <col min="4" width="9.10" max="4"/>
+    <col min="3" width="9.10" max="3"/>
+    <col min="2" width="9.10" max="2"/>
+    <col min="1" width="9.10" max="1"/>
+    <col min="15" width="9.10" max="15"/>
+    <col min="14" width="9.10" max="14"/>
+    <col min="13" width="9.10" max="13"/>
+    <col min="12" width="9.10" max="12"/>
+    <col min="11" width="9.10" max="11"/>
+    <col min="10" width="9.10" max="10"/>
+    <col min="9" width="9.10" max="9"/>
+    <col min="8" width="9.10" max="8"/>
+    <col min="23" width="9.10" max="23"/>
+    <col min="22" width="9.10" max="22"/>
+    <col min="21" width="9.10" max="21"/>
+    <col min="20" width="9.10" max="20"/>
+    <col min="19" width="9.10" max="19"/>
+    <col min="18" width="9.10" max="18"/>
+    <col min="17" width="9.10" max="17"/>
+    <col min="16" width="9.10" max="16"/>
+    <col min="24" width="9.10" max="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">

</xml_diff>